<commit_message>
Stoney nearly Finished + Axe adds to inventory when removed from Stoney
</commit_message>
<xml_diff>
--- a/Planing/Guppen-Planung.xlsx
+++ b/Planing/Guppen-Planung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -136,13 +136,16 @@
     <t>Bugfixing</t>
   </si>
   <si>
-    <t>Bugfixing siehe Bugs.xlsx</t>
-  </si>
-  <si>
     <t>Sprite für Springen</t>
   </si>
   <si>
-    <t>Ax in the Stone for Cave</t>
+    <t>Axe in the Stone for Cave</t>
+  </si>
+  <si>
+    <t>Helth UI for Enemies</t>
+  </si>
+  <si>
+    <t>Bugfixing siehe Bugs.xlsx Didn't fixed all Bugs</t>
   </si>
 </sst>
 </file>
@@ -383,9 +386,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +426,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -495,7 +498,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -672,7 +675,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,21 +1302,23 @@
       <c r="C21" s="1">
         <v>6</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -1327,29 +1332,31 @@
       <c r="C22" s="1">
         <v>3</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
@@ -1377,43 +1384,61 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="4">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H24" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>✔</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="B25" s="4">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>✔</v>
       </c>
       <c r="I25" s="1"/>
     </row>

</xml_diff>